<commit_message>
add web scrape example
</commit_message>
<xml_diff>
--- a/schedule_685.xlsx
+++ b/schedule_685.xlsx
@@ -1,28 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/math_685/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math_685\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45320AC-031E-8A4B-AD44-D33A12AA9422}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07DB21F-41ED-4771-9137-2567512AD9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="slo_detail" sheetId="5" r:id="rId1"/>
+    <sheet name="Weekly Detail" sheetId="5" r:id="rId1"/>
+    <sheet name="Learning Resources" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">slo_detail!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Weekly Detail'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="83">
   <si>
     <t>Finals Week</t>
   </si>
@@ -170,15 +179,6 @@
     <t xml:space="preserve">Dissemination to a broader public. </t>
   </si>
   <si>
-    <t>Web scraping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not all data comes in tables. </t>
-  </si>
-  <si>
-    <t>rvest, XML</t>
-  </si>
-  <si>
     <t>Clustering methods</t>
   </si>
   <si>
@@ -192,12 +192,6 @@
   </si>
   <si>
     <t>Bootstrapping</t>
-  </si>
-  <si>
-    <t>twitter, regex hell, stringr, word clouds, sentiment analysis</t>
-  </si>
-  <si>
-    <t>API, text processing, sentiment analysis</t>
   </si>
   <si>
     <t>Unsupervised learning / dimension reduction</t>
@@ -254,14 +248,87 @@
     <t>Get data from the web</t>
   </si>
   <si>
-    <t>Stat 545: Get data from the web https://stat545.com/web-data-slides.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">Data is everywhere. How can we get our hands on it? 
 Data also comes by way of different delivery systems also. </t>
   </si>
   <si>
     <t>functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stat 545: Get data from the web Ch 39
+</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>date accessed</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://regex101.com</t>
+  </si>
+  <si>
+    <t>sub-topic</t>
+  </si>
+  <si>
+    <t>regex</t>
+  </si>
+  <si>
+    <t>stringr</t>
+  </si>
+  <si>
+    <t>https://stringr.tidyverse.org/index.html</t>
+  </si>
+  <si>
+    <t>text analysis</t>
+  </si>
+  <si>
+    <t>text processing</t>
+  </si>
+  <si>
+    <t>web scraping</t>
+  </si>
+  <si>
+    <t>rvest</t>
+  </si>
+  <si>
+    <t>https://blog.rsquaredacademy.com/web-scraping/</t>
+  </si>
+  <si>
+    <t>https://cfss.uchicago.edu/notes/web-scraping/#html</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>amazing tool to figure out how to write regexpressions</t>
+  </si>
+  <si>
+    <t>General tutorial</t>
+  </si>
+  <si>
+    <t>https://cfss.uchicago.edu</t>
+  </si>
+  <si>
+    <t>https://blog.rsquaredacademy.com/</t>
+  </si>
+  <si>
+    <t>https://stat545.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data is out there. How can you use it to tell a compelling story? Or to enhance your own story? </t>
+  </si>
+  <si>
+    <t>word clouds, sentiment analysis</t>
+  </si>
+  <si>
+    <t>regex hell, stringr</t>
+  </si>
+  <si>
+    <t>Analyze twitter data for days during campfire. Present at anniversary.</t>
   </si>
 </sst>
 </file>
@@ -271,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,7 +411,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,6 +442,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -482,7 +555,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -555,6 +628,25 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="79"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="79" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="80">
@@ -974,26 +1066,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="51" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="3" customWidth="1"/>
-    <col min="4" max="7" width="36.83203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="36.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="2.83203125" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="88.6640625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="14.83203125" style="3"/>
+    <col min="1" max="1" width="7.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.625" style="3" customWidth="1"/>
+    <col min="4" max="7" width="36.875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="2.875" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="88.625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="14.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1022,7 +1114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="208">
+    <row r="2" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1049,10 +1141,10 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="80">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1074,14 +1166,14 @@
         <v>16</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="64">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1107,7 +1199,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="80">
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1133,7 +1225,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="256">
+    <row r="6" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1151,20 +1243,20 @@
         <v>35</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1180,7 +1272,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="64">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1204,8 +1296,8 @@
       <c r="H8" s="14"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="44" customHeight="1">
-      <c r="A9" s="18">
+    <row r="9" spans="1:10" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>8</v>
       </c>
       <c r="B9" s="13">
@@ -1218,12 +1310,12 @@
       <c r="F9" s="15"/>
       <c r="G9" s="14"/>
       <c r="H9" s="16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="64">
-      <c r="A10" s="18">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="B10" s="13">
@@ -1231,20 +1323,22 @@
         <v>42297</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="H10" s="19"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="29" customHeight="1">
+    <row r="11" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -1252,19 +1346,21 @@
         <f t="shared" si="0"/>
         <v>42304</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>47</v>
+      <c r="C11" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
-        <v>46</v>
+      <c r="E11" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="31" t="s">
+        <v>82</v>
+      </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="29" customHeight="1">
+    <row r="12" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -1272,15 +1368,19 @@
         <f t="shared" si="0"/>
         <v>42311</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="C12" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="19"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="29" customHeight="1">
+    <row r="13" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -1294,11 +1394,11 @@
       <c r="F13" s="20"/>
       <c r="G13" s="14"/>
       <c r="H13" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="29" customHeight="1">
+    <row r="14" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -1307,7 +1407,7 @@
         <v>42325</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -1316,7 +1416,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="29" customHeight="1">
+    <row r="15" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="13">
         <f t="shared" si="0"/>
@@ -1330,7 +1430,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="39" customHeight="1">
+    <row r="16" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>14</v>
       </c>
@@ -1339,18 +1439,18 @@
         <v>42339</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="19"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="29" customHeight="1">
+    <row r="17" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>15</v>
       </c>
@@ -1359,18 +1459,18 @@
         <v>42346</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="19"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="29" customHeight="1">
+    <row r="18" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>0</v>
       </c>
@@ -1386,25 +1486,25 @@
       <c r="H18" s="19"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="29" customHeight="1">
+    <row r="19" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="23"/>
       <c r="C19" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="29" customHeight="1">
+    <row r="20" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="23"/>
       <c r="C20" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -1412,33 +1512,163 @@
       <c r="G20" s="15"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="29" customHeight="1">
+    <row r="21" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="29" customHeight="1">
-      <c r="C22" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="29" customHeight="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D29" s="25"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G6" r:id="rId1" display="https://holtzy.github.io/Pimp-my-rmd/" xr:uid="{8AF682AA-9264-40B5-90D7-3FF02F13B3B5}"/>
-    <hyperlink ref="E10" r:id="rId2" xr:uid="{0F2B4E34-455B-9E48-B1D6-B198CFE5C1EC}"/>
+    <hyperlink ref="E10" r:id="rId2" display="Stat 545: Get data from the web https://stat545.com/web-data-slides.html" xr:uid="{0F2B4E34-455B-9E48-B1D6-B198CFE5C1EC}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="85" orientation="landscape" blackAndWhite="1" draft="1" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A793E651-852A-4512-B8D0-B3343307CB94}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="26"/>
+    <col min="3" max="3" width="12.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="18.625" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="28">
+        <v>42300</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="28">
+        <v>42300</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="28">
+        <v>42300</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="28">
+        <v>42300</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="28">
+        <v>42300</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="28">
+        <v>42300</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="28">
+        <v>42300</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="https://regex101.com/" xr:uid="{9E1A45EF-B303-4D59-9F08-BBB2ADD4CB89}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{1C85CB35-4CBA-4A89-857E-E37418094E26}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{AA085BCF-0942-4324-ADBB-DEDA2B9B10E2}"/>
+    <hyperlink ref="E5" r:id="rId4" location="html" display="https://cfss.uchicago.edu/notes/web-scraping/ - html" xr:uid="{062B566B-ABC8-4503-BC9C-ADAE7F5E64BC}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{20FCD814-90F1-4E89-81CF-F4DFB65D8CEB}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{194F93BF-98DB-4706-AD44-18216FE6D52A}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{E3B96E83-8C7F-4BA3-AF39-5097862C1F77}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>